<commit_message>
Fixed an error in Japan scaling mapping file.
</commit_message>
<xml_diff>
--- a/input/mappings/scaling/jpn_scaling_mapping.xlsx
+++ b/input/mappings/scaling/jpn_scaling_mapping.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26929"/>
-  <workbookPr autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="10800" yWindow="5040" windowWidth="22660" windowHeight="14000" activeTab="2"/>
+    <workbookView xWindow="10800" yWindow="5040" windowWidth="22665" windowHeight="13620"/>
   </bookViews>
   <sheets>
     <sheet name="map" sheetId="1" r:id="rId1"/>
     <sheet name="method" sheetId="2" r:id="rId2"/>
     <sheet name="year" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="140001"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -942,23 +942,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D65"/>
+  <dimension ref="A1:D66"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A23" sqref="A23"/>
+      <selection pane="bottomRight" activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.33203125" customWidth="1"/>
-    <col min="2" max="2" width="39.5" customWidth="1"/>
-    <col min="3" max="3" width="40.33203125" customWidth="1"/>
+    <col min="1" max="1" width="30.28515625" customWidth="1"/>
+    <col min="2" max="2" width="39.42578125" customWidth="1"/>
+    <col min="3" max="3" width="40.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>58</v>
       </c>
@@ -970,7 +970,7 @@
       </c>
       <c r="D1" s="1"/>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>54</v>
       </c>
@@ -982,16 +982,16 @@
       </c>
       <c r="D2" s="3"/>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>0</v>
+        <v>54</v>
       </c>
       <c r="C3" t="s">
         <v>0</v>
       </c>
       <c r="D3" s="3"/>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>54</v>
       </c>
@@ -999,7 +999,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -1010,7 +1010,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -1021,7 +1021,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -1032,7 +1032,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -1043,7 +1043,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -1054,7 +1054,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -1065,7 +1065,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -1076,7 +1076,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -1087,7 +1087,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -1098,7 +1098,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -1109,7 +1109,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -1120,7 +1120,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -1131,7 +1131,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -1142,7 +1142,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -1150,7 +1150,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -1158,7 +1158,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -1169,7 +1169,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -1180,7 +1180,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>20</v>
       </c>
@@ -1188,7 +1188,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>73</v>
       </c>
@@ -1196,7 +1196,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>21</v>
       </c>
@@ -1207,7 +1207,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>22</v>
       </c>
@@ -1218,7 +1218,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>23</v>
       </c>
@@ -1229,7 +1229,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>24</v>
       </c>
@@ -1240,53 +1240,42 @@
         <v>24</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
-      <c r="A28" t="s">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>9</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B29" t="s">
         <v>70</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C29" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
-      <c r="A29" t="s">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>25</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B30" t="s">
         <v>25</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C30" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
-      <c r="A30" t="s">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>26</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B31" t="s">
         <v>26</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C31" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="31" spans="1:3">
-      <c r="A31" t="s">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>55</v>
-      </c>
-      <c r="B31" t="s">
-        <v>27</v>
-      </c>
-      <c r="C31" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3">
-      <c r="A32" t="s">
-        <v>51</v>
       </c>
       <c r="B32" t="s">
         <v>27</v>
@@ -1295,9 +1284,9 @@
         <v>27</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B33" t="s">
         <v>27</v>
@@ -1306,75 +1295,75 @@
         <v>27</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
+        <v>56</v>
+      </c>
+      <c r="B34" t="s">
+        <v>27</v>
+      </c>
+      <c r="C34" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>28</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B35" t="s">
         <v>28</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C35" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="35" spans="1:3">
-      <c r="A35" t="s">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>29</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B36" t="s">
         <v>29</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C36" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
-      <c r="A36" t="s">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>30</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B37" t="s">
         <v>30</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C37" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="37" spans="1:3">
-      <c r="A37" t="s">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>31</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B38" t="s">
         <v>31</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C38" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="38" spans="1:3">
-      <c r="A38" t="s">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>32</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B39" t="s">
         <v>32</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C39" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="39" spans="1:3">
-      <c r="A39" s="1" t="s">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="B39" t="s">
-        <v>33</v>
-      </c>
-      <c r="C39" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3">
-      <c r="A40" s="1" t="s">
-        <v>53</v>
       </c>
       <c r="B40" t="s">
         <v>33</v>
@@ -1383,9 +1372,9 @@
         <v>33</v>
       </c>
     </row>
-    <row r="41" spans="1:3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B41" t="s">
         <v>33</v>
@@ -1394,221 +1383,232 @@
         <v>33</v>
       </c>
     </row>
-    <row r="42" spans="1:3">
-      <c r="A42" t="s">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B42" t="s">
+        <v>33</v>
+      </c>
+      <c r="C42" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
         <v>34</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B43" t="s">
         <v>34</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C43" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="43" spans="1:3">
-      <c r="A43" t="s">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
         <v>36</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B44" t="s">
         <v>36</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C44" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="44" spans="1:3">
-      <c r="A44" s="1" t="s">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B45" t="s">
         <v>37</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C45" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="45" spans="1:3">
-      <c r="A45" s="1" t="s">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B46" t="s">
         <v>35</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C46" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="46" spans="1:3">
-      <c r="A46" s="1" t="s">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B47" t="s">
         <v>38</v>
       </c>
-      <c r="C46" t="s">
+      <c r="C47" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="47" spans="1:3">
-      <c r="A47" s="1" t="s">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B48" t="s">
         <v>39</v>
       </c>
-      <c r="C47" t="s">
+      <c r="C48" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="48" spans="1:3">
-      <c r="A48" s="1" t="s">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B49" t="s">
         <v>40</v>
       </c>
-      <c r="C48" t="s">
+      <c r="C49" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="49" spans="1:3">
-      <c r="A49" s="1" t="s">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B50" t="s">
         <v>41</v>
       </c>
-      <c r="C49" t="s">
+      <c r="C50" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="50" spans="1:3">
-      <c r="A50" s="1" t="s">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B51" t="s">
         <v>42</v>
       </c>
-      <c r="C50" t="s">
+      <c r="C51" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="51" spans="1:3">
-      <c r="A51" s="1" t="s">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B51" s="1" t="s">
+      <c r="B52" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C51" t="s">
+      <c r="C52" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="52" spans="1:3">
-      <c r="A52" s="1" t="s">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B52" s="1" t="s">
+      <c r="B53" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C52" t="s">
+      <c r="C53" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="53" spans="1:3">
-      <c r="A53" s="1" t="s">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B53" s="1" t="s">
+      <c r="B54" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C53" t="s">
+      <c r="C54" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="54" spans="1:3">
-      <c r="A54" s="1" t="s">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B54" s="1" t="s">
+      <c r="B55" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C54" t="s">
+      <c r="C55" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="55" spans="1:3">
-      <c r="A55" s="1" t="s">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B55" s="1" t="s">
+      <c r="B56" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C55" t="s">
+      <c r="C56" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="56" spans="1:3">
-      <c r="A56" s="1" t="s">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B56" s="1" t="s">
+      <c r="B57" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C56" t="s">
+      <c r="C57" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="57" spans="1:3">
-      <c r="A57" s="1" t="s">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B57" s="1" t="s">
+      <c r="B58" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C57" t="s">
+      <c r="C58" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="58" spans="1:3">
-      <c r="A58" s="1" t="s">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B58" s="1" t="s">
+      <c r="B59" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C58" t="s">
+      <c r="C59" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="59" spans="1:3">
-      <c r="A59" s="1" t="s">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B60" t="s">
         <v>50</v>
       </c>
-      <c r="C59" t="s">
+      <c r="C60" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="60" spans="1:3">
-      <c r="A60" s="1"/>
-    </row>
-    <row r="61" spans="1:3">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="1"/>
     </row>
-    <row r="62" spans="1:3">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="1"/>
     </row>
-    <row r="63" spans="1:3">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="1"/>
     </row>
-    <row r="64" spans="1:3">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
     </row>
-    <row r="65" spans="1:1">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" s="1"/>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1629,9 +1629,9 @@
       <selection sqref="A1:E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>61</v>
       </c>
@@ -1648,7 +1648,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>65</v>
       </c>
@@ -1679,13 +1679,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" ht="15">
+    <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>61</v>
       </c>
@@ -1699,7 +1699,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>65</v>
       </c>

</xml_diff>